<commit_message>
updates everything to most recent 12S and 16S outputs and cleans up code flow
</commit_message>
<xml_diff>
--- a/Deliverables/12S/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies-4.xlsx
+++ b/Deliverables/12S/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies-4.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/Deliverables/12S/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_A6239EC68F79A8D366075C52F37BD2722AC6C29E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18AF8912-610B-40BC-9B80-E83E19972543}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="11_A6239EC68F79A8D366075C52F37BD2722AC6C29E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37DBE1AD-4A31-499A-808A-289C8A615A64}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
-    <sheet name="no_Mammals" sheetId="2" r:id="rId2"/>
+    <sheet name="no_Mammals.Bact" sheetId="2" r:id="rId2"/>
     <sheet name="Unassigned" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4013" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4018" uniqueCount="451">
   <si>
     <t>rownames</t>
   </si>
@@ -1360,6 +1360,21 @@
   </si>
   <si>
     <t>TATACGAGAGGCCCAAATTGATGAAAAACGGCGTAAAGCGTGTTAAAGATCAGCCCACACTAAAGCTAAAACCTAACCAAGCCGTAAAAAGCTACCGTTAACATAAAATAAACCACCAACGTGACTTTACTAATTCTGACTGCACGATACCTAAG</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>&gt;99% Eleginus gracilis, Microgradus proximus</t>
+  </si>
+  <si>
+    <t>&gt;99% Myoxocephalus stelleri, Myoxocephalus jaok, Myoxocephalus polyacanthocephalus</t>
+  </si>
+  <si>
+    <t>100% Myoxocephalus scorpius, Myoxocephalus quadricornis, Myoxocephalus aenaeus</t>
+  </si>
+  <si>
+    <t>&gt;99% Myoxocephalus scorpius, Megalocottus platycephalus, Myoxocephalus quadricornis, Myoxocephalus aenaeus</t>
   </si>
 </sst>
 </file>
@@ -1423,6 +1438,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1714,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J290"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="A256" sqref="A256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9096,7 +9115,7 @@
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
@@ -14114,10 +14133,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91819D1C-3F26-4D97-97AC-D8458771B1EC}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14133,7 +14152,7 @@
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14164,8 +14183,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -14190,8 +14212,11 @@
       <c r="I2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -14210,8 +14235,11 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -14233,8 +14261,11 @@
       <c r="G4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -14256,8 +14287,11 @@
       <c r="G5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -14283,7 +14317,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -14309,7 +14343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -14332,7 +14366,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>160</v>
       </c>
@@ -14352,7 +14386,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -14372,7 +14406,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -14383,12 +14417,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>207</v>
       </c>
@@ -14408,7 +14442,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>209</v>
       </c>
@@ -14428,7 +14462,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>221</v>
       </c>
@@ -14439,7 +14473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>226</v>
       </c>

</xml_diff>

<commit_message>
for 12s and 16s: removes samples with fewer than 100 reads; compares and removes replicates; fills in NA species with ASV names; removes unassigned sequences. For 12s: removes Melanogrammus aeglefinus from 12S reference database and reruns dada2. Updates all deliverables for 12s and 16s
</commit_message>
<xml_diff>
--- a/Deliverables/12S/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies-4.xlsx
+++ b/Deliverables/12S/WADE003-arcticpred_dada2_QAQC_12SP1_output-addspecies-4.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="49" documentId="11_A6239EC68F79A8D366075C52F37BD2722AC6C29E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37DBE1AD-4A31-499A-808A-289C8A615A64}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -1438,10 +1438,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1733,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J290"/>
   <sheetViews>
-    <sheetView topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="A256" sqref="A256"/>
+    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="J239" sqref="J239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14135,7 +14131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91819D1C-3F26-4D97-97AC-D8458771B1EC}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>

</xml_diff>